<commit_message>
Added functionality of excel mapper, last commits failed
</commit_message>
<xml_diff>
--- a/Java Backend/data/University Courses POC.xlsx
+++ b/Java Backend/data/University Courses POC.xlsx
@@ -8,17 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/815b8c016bd40a6d/Projects/Youni/Youni/Java Backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="217" documentId="11_F25DC773A252ABDACC10487EC99B6D305ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{76DCD41F-4824-4274-9D0C-09103A343694}"/>
+  <xr:revisionPtr revIDLastSave="244" documentId="11_F25DC773A252ABDACC10487EC99B6D305ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36824758-D513-462A-83D8-89A1A05A0B89}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -51,9 +62,6 @@
     <t>Degree Type</t>
   </si>
   <si>
-    <t>Required Letters</t>
-  </si>
-  <si>
     <t>Required Grades Upper</t>
   </si>
   <si>
@@ -223,6 +231,9 @@
   </si>
   <si>
     <t>Rec Type 5</t>
+  </si>
+  <si>
+    <t>Required IB</t>
   </si>
 </sst>
 </file>
@@ -258,8 +269,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -546,8 +558,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,10 +576,8 @@
     <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="16" customWidth="1"/>
-    <col min="14" max="14" width="7.42578125" customWidth="1"/>
-    <col min="15" max="16" width="14.42578125" customWidth="1"/>
-    <col min="17" max="17" width="7.42578125" customWidth="1"/>
-    <col min="18" max="19" width="14.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="19" width="14.42578125" customWidth="1"/>
     <col min="20" max="20" width="7.42578125" customWidth="1"/>
     <col min="21" max="22" width="14.42578125" customWidth="1"/>
     <col min="23" max="23" width="7.42578125" customWidth="1"/>
@@ -596,67 +606,67 @@
         <v>7</v>
       </c>
       <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
-        <v>13</v>
-      </c>
       <c r="M1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" t="s">
         <v>21</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>31</v>
+      </c>
+      <c r="P1" t="s">
         <v>22</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
+        <v>23</v>
+      </c>
+      <c r="R1" t="s">
         <v>32</v>
       </c>
-      <c r="P1" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>24</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" t="s">
-        <v>25</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>26</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" t="s">
         <v>34</v>
       </c>
-      <c r="V1" t="s">
-        <v>27</v>
-      </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>28</v>
       </c>
-      <c r="X1" t="s">
-        <v>35</v>
-      </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>29</v>
       </c>
-      <c r="Z1" t="s">
-        <v>30</v>
-      </c>
       <c r="AA1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -666,53 +676,53 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="1">
         <v>25</v>
       </c>
       <c r="D2" t="s">
         <v>3</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="1">
         <v>3</v>
       </c>
       <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>16</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" t="s">
         <v>37</v>
       </c>
-      <c r="K2" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
+        <v>30</v>
+      </c>
+      <c r="R2" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" t="s">
         <v>38</v>
       </c>
-      <c r="P2" t="s">
-        <v>31</v>
-      </c>
-      <c r="R2" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" t="s">
-        <v>39</v>
-      </c>
       <c r="U2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -720,43 +730,43 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1">
+        <v>33</v>
+      </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" t="s">
         <v>41</v>
       </c>
-      <c r="C3">
-        <v>33</v>
-      </c>
-      <c r="D3" t="s">
-        <v>40</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>42</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
         <v>43</v>
       </c>
-      <c r="J3" t="s">
-        <v>37</v>
-      </c>
-      <c r="K3" t="s">
-        <v>44</v>
-      </c>
       <c r="L3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -764,43 +774,43 @@
         <v>1</v>
       </c>
       <c r="B4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1">
+        <v>20</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
         <v>45</v>
       </c>
-      <c r="C4">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
         <v>46</v>
       </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" t="s">
-        <v>47</v>
-      </c>
       <c r="L4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
@@ -808,252 +818,252 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="1">
+        <v>26</v>
+      </c>
+      <c r="D5" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" t="s">
         <v>48</v>
       </c>
-      <c r="C5">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5" t="s">
+      <c r="H5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>49</v>
       </c>
-      <c r="H5" t="s">
-        <v>15</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
         <v>50</v>
       </c>
-      <c r="J5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" t="s">
-        <v>51</v>
-      </c>
       <c r="L5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="1">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
+      <c r="H6" t="s">
         <v>52</v>
       </c>
-      <c r="B6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6">
-        <v>2</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6">
-        <v>3</v>
-      </c>
-      <c r="F6" t="s">
-        <v>46</v>
-      </c>
-      <c r="H6" t="s">
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>17</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6" t="s">
+        <v>19</v>
+      </c>
+      <c r="N6" t="s">
+        <v>54</v>
+      </c>
+      <c r="O6" t="s">
+        <v>35</v>
+      </c>
+      <c r="P6" t="s">
         <v>53</v>
       </c>
-      <c r="J6" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" t="s">
-        <v>18</v>
-      </c>
-      <c r="L6" t="s">
-        <v>19</v>
-      </c>
-      <c r="M6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N6" t="s">
-        <v>55</v>
-      </c>
-      <c r="O6" t="s">
-        <v>36</v>
-      </c>
-      <c r="P6" t="s">
-        <v>54</v>
-      </c>
       <c r="R6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="S6" t="s">
         <v>3</v>
       </c>
       <c r="U6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="1">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3</v>
+      </c>
+      <c r="F7" t="s">
+        <v>45</v>
+      </c>
+      <c r="H7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E7">
-        <v>3</v>
-      </c>
-      <c r="F7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H7" t="s">
-        <v>53</v>
-      </c>
       <c r="J7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" t="s">
+        <v>55</v>
+      </c>
+      <c r="L7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7" t="s">
+        <v>39</v>
+      </c>
+      <c r="O7" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" t="s">
+        <v>56</v>
+      </c>
+      <c r="R7" t="s">
+        <v>37</v>
+      </c>
+      <c r="S7" t="s">
+        <v>38</v>
+      </c>
+      <c r="U7" t="s">
+        <v>37</v>
+      </c>
+      <c r="V7" t="s">
         <v>19</v>
       </c>
-      <c r="K7" t="s">
-        <v>56</v>
-      </c>
-      <c r="L7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M7" t="s">
-        <v>40</v>
-      </c>
-      <c r="O7" t="s">
-        <v>36</v>
-      </c>
-      <c r="P7" t="s">
+      <c r="X7" t="s">
         <v>57</v>
-      </c>
-      <c r="R7" t="s">
-        <v>38</v>
-      </c>
-      <c r="S7" t="s">
-        <v>39</v>
-      </c>
-      <c r="U7" t="s">
-        <v>38</v>
-      </c>
-      <c r="V7" t="s">
-        <v>20</v>
-      </c>
-      <c r="X7" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3</v>
+      </c>
+      <c r="F8" t="s">
         <v>45</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="H8" t="s">
+        <v>48</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>46</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8" t="s">
         <v>59</v>
       </c>
-      <c r="E8">
-        <v>3</v>
-      </c>
-      <c r="F8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" t="s">
-        <v>49</v>
-      </c>
-      <c r="J8" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" t="s">
-        <v>47</v>
-      </c>
-      <c r="L8" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" t="s">
+      <c r="O8" t="s">
+        <v>37</v>
+      </c>
+      <c r="P8" t="s">
         <v>60</v>
       </c>
-      <c r="O8" t="s">
-        <v>38</v>
-      </c>
-      <c r="P8" t="s">
-        <v>61</v>
-      </c>
       <c r="R8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="1">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+      <c r="H9" t="s">
         <v>52</v>
       </c>
-      <c r="B9" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="J9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s">
         <v>62</v>
       </c>
-      <c r="E9">
-        <v>3</v>
-      </c>
-      <c r="F9" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" t="s">
-        <v>53</v>
-      </c>
-      <c r="J9" t="s">
+      <c r="L9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9" t="s">
+        <v>47</v>
+      </c>
+      <c r="O9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P9" t="s">
         <v>19</v>
       </c>
-      <c r="K9" t="s">
+      <c r="R9" t="s">
         <v>63</v>
       </c>
-      <c r="L9" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" t="s">
-        <v>48</v>
-      </c>
-      <c r="O9" t="s">
-        <v>64</v>
-      </c>
-      <c r="P9" t="s">
-        <v>20</v>
-      </c>
-      <c r="R9" t="s">
-        <v>64</v>
-      </c>
       <c r="S9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="V9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="X9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="Y9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed last couple of bugs for the upload
</commit_message>
<xml_diff>
--- a/Java Backend/data/University Courses POC.xlsx
+++ b/Java Backend/data/University Courses POC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/815b8c016bd40a6d/Projects/Youni/Youni/Java Backend/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="244" documentId="11_F25DC773A252ABDACC10487EC99B6D305ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36824758-D513-462A-83D8-89A1A05A0B89}"/>
+  <xr:revisionPtr revIDLastSave="250" documentId="11_F25DC773A252ABDACC10487EC99B6D305ADE58EA" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E71E813A-ABCA-4B50-B3CE-46066B3476FA}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="66">
   <si>
     <t>University Name</t>
   </si>
@@ -209,9 +209,6 @@
     <t>Chemistry</t>
   </si>
   <si>
-    <t>Mutliple</t>
-  </si>
-  <si>
     <t>English Literature and Language</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t>Required IB</t>
+  </si>
+  <si>
+    <t>null</t>
   </si>
 </sst>
 </file>
@@ -276,7 +276,15 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -558,8 +566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="Z25" sqref="Z25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,7 +620,7 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J1" t="s">
         <v>10</v>
@@ -666,7 +674,7 @@
         <v>29</v>
       </c>
       <c r="AA1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.25">
@@ -709,20 +717,47 @@
       <c r="M2" t="s">
         <v>19</v>
       </c>
+      <c r="N2" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="O2" t="s">
         <v>37</v>
       </c>
       <c r="P2" t="s">
         <v>30</v>
       </c>
+      <c r="Q2" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="R2" t="s">
         <v>37</v>
       </c>
       <c r="S2" t="s">
         <v>38</v>
       </c>
+      <c r="T2" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="U2" t="s">
         <v>37</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.25">
@@ -765,8 +800,47 @@
       <c r="M3" t="s">
         <v>39</v>
       </c>
+      <c r="N3" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="O3" t="s">
         <v>35</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:27" x14ac:dyDescent="0.25">
@@ -809,8 +883,47 @@
       <c r="M4" t="s">
         <v>44</v>
       </c>
+      <c r="N4" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="O4" t="s">
         <v>35</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.25">
@@ -850,6 +963,51 @@
       <c r="L5" t="s">
         <v>18</v>
       </c>
+      <c r="M5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z5" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -870,9 +1028,15 @@
       <c r="F6" t="s">
         <v>45</v>
       </c>
+      <c r="G6" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="H6" t="s">
         <v>52</v>
       </c>
+      <c r="I6" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="J6" t="s">
         <v>18</v>
       </c>
@@ -894,14 +1058,38 @@
       <c r="P6" t="s">
         <v>53</v>
       </c>
+      <c r="Q6" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="R6" t="s">
         <v>37</v>
       </c>
       <c r="S6" t="s">
         <v>3</v>
       </c>
+      <c r="T6" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="U6" t="s">
         <v>37</v>
+      </c>
+      <c r="V6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA6" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.25">
@@ -923,9 +1111,15 @@
       <c r="F7" t="s">
         <v>45</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="H7" t="s">
         <v>52</v>
       </c>
+      <c r="I7" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="J7" t="s">
         <v>18</v>
       </c>
@@ -938,26 +1132,47 @@
       <c r="M7" t="s">
         <v>39</v>
       </c>
+      <c r="N7" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="O7" t="s">
         <v>35</v>
       </c>
       <c r="P7" t="s">
         <v>56</v>
       </c>
+      <c r="Q7" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="R7" t="s">
         <v>37</v>
       </c>
       <c r="S7" t="s">
         <v>38</v>
       </c>
+      <c r="T7" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="U7" t="s">
         <v>37</v>
       </c>
       <c r="V7" t="s">
         <v>19</v>
       </c>
+      <c r="W7" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="X7" t="s">
-        <v>57</v>
+        <v>37</v>
+      </c>
+      <c r="Y7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA7" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="8" spans="1:27" x14ac:dyDescent="0.25">
@@ -971,7 +1186,7 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E8" s="1">
         <v>3</v>
@@ -979,9 +1194,15 @@
       <c r="F8" t="s">
         <v>45</v>
       </c>
+      <c r="G8" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="H8" t="s">
         <v>48</v>
       </c>
+      <c r="I8" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="J8" t="s">
         <v>18</v>
       </c>
@@ -992,16 +1213,49 @@
         <v>18</v>
       </c>
       <c r="M8" t="s">
-        <v>59</v>
+        <v>58</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="O8" t="s">
         <v>37</v>
       </c>
       <c r="P8" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="Q8" s="1" t="s">
+        <v>65</v>
       </c>
       <c r="R8" t="s">
         <v>37</v>
+      </c>
+      <c r="S8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="U8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="X8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Y8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="AA8" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.25">
@@ -1015,7 +1269,7 @@
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E9" s="1">
         <v>3</v>
@@ -1023,14 +1277,20 @@
       <c r="F9" t="s">
         <v>45</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="H9" t="s">
         <v>52</v>
       </c>
+      <c r="I9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="J9" t="s">
         <v>18</v>
       </c>
       <c r="K9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L9" t="s">
         <v>18</v>
@@ -1038,35 +1298,55 @@
       <c r="M9" t="s">
         <v>47</v>
       </c>
+      <c r="N9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="O9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P9" t="s">
         <v>19</v>
       </c>
+      <c r="Q9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="R9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S9" t="s">
         <v>39</v>
       </c>
+      <c r="T9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="U9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V9" t="s">
         <v>38</v>
       </c>
+      <c r="W9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="X9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Y9" t="s">
         <v>56</v>
       </c>
+      <c r="Z9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="AA9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="A2:AA9">
+    <cfRule type="containsBlanks" dxfId="0" priority="1">
+      <formula>LEN(TRIM(A2))=0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>